<commit_message>
Added the rest of the progress to the slides
</commit_message>
<xml_diff>
--- a/Database example.xlsx
+++ b/Database example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rawso\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rawso\Desktop\nwen\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A445AB4B-60C9-4F8F-BA49-F34244BBD6CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDDDF1A-6CF9-4FAC-ADAB-3E389DC81713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>ISBN</t>
   </si>
@@ -72,18 +72,9 @@
     <t>Price</t>
   </si>
   <si>
-    <t>No. of visitors</t>
-  </si>
-  <si>
-    <t>No. bought</t>
-  </si>
-  <si>
     <t>Table for Users</t>
   </si>
   <si>
-    <t>Table for Products</t>
-  </si>
-  <si>
     <t>User ID</t>
   </si>
   <si>
@@ -114,22 +105,19 @@
     <t>double</t>
   </si>
   <si>
-    <t>Image Link</t>
-  </si>
-  <si>
     <t>InStock</t>
   </si>
   <si>
-    <t>Purchase History</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>NumSold</t>
+  </si>
+  <si>
+    <t>Table for Books</t>
+  </si>
+  <si>
+    <t>No. of veiws</t>
+  </si>
+  <si>
+    <t>Image source</t>
   </si>
 </sst>
 </file>
@@ -475,15 +463,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
@@ -491,16 +479,17 @@
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -520,7 +509,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -532,19 +521,16 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -561,7 +547,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -576,50 +562,47 @@
         <v>13</v>
       </c>
       <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -630,52 +613,19 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the book list and the images
</commit_message>
<xml_diff>
--- a/Database example.xlsx
+++ b/Database example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rawso\Desktop\nwen\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDDDF1A-6CF9-4FAC-ADAB-3E389DC81713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37F9D79-1E90-4C07-8C58-093DF5C9D07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>ISBN</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Activity History</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>InStock</t>
   </si>
   <si>
@@ -118,6 +115,12 @@
   </si>
   <si>
     <t>Image source</t>
+  </si>
+  <si>
+    <t>float8</t>
+  </si>
+  <si>
+    <t>Primary Key</t>
   </si>
 </sst>
 </file>
@@ -466,18 +469,19 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -486,7 +490,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -509,7 +516,7 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -521,13 +528,13 @@
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
         <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -547,7 +554,7 @@
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -562,7 +569,7 @@
         <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" t="s">
         <v>9</v>

</xml_diff>